<commit_message>
Added remote64-controller firmware source.
</commit_message>
<xml_diff>
--- a/controller/pinout.xlsx
+++ b/controller/pinout.xlsx
@@ -163,7 +163,7 @@
     <t xml:space="preserve">RD4</t>
   </si>
   <si>
-    <t xml:space="preserve">UART2 RX</t>
+    <t xml:space="preserve">UART1 RX</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Controller 4</t>
   </si>
   <si>
-    <t xml:space="preserve">UART2 TX</t>
+    <t xml:space="preserve">UART1 TX</t>
   </si>
   <si>
     <t xml:space="preserve">UART_TX</t>
@@ -556,7 +556,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>